<commit_message>
- Add IO files. - Send PN to PLC - Station 8 Full sequance. (Remove NG sensors.)
</commit_message>
<xml_diff>
--- a/MemoryMap/IO_Mapping_Misubishi_Profinet(IFM).xlsx
+++ b/MemoryMap/IO_Mapping_Misubishi_Profinet(IFM).xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F3377F-81D6-4EA3-92DB-199C8647EC4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master1 Mapping" sheetId="6" r:id="rId1"/>
     <sheet name="Dia" sheetId="16" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -703,8 +704,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,7 +722,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,6 +756,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -834,6 +841,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -877,7 +887,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -926,7 +942,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Straight Connector 5"/>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -975,7 +997,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Connector 7"/>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1024,7 +1052,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1316,21 +1350,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
@@ -1341,7 +1375,7 @@
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1401,7 @@
       <c r="T1" s="10"/>
       <c r="U1" s="10"/>
     </row>
-    <row r="2" spans="2:24">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1454,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>223</v>
       </c>
@@ -1470,7 +1504,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>224</v>
       </c>
@@ -1492,10 +1526,10 @@
       <c r="K4" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="14" t="s">
         <v>179</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -1520,7 +1554,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>93</v>
       </c>
@@ -1542,13 +1576,13 @@
       <c r="K5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="14" t="s">
         <v>182</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="14" t="s">
         <v>180</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -1570,7 +1604,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>94</v>
       </c>
@@ -1620,7 +1654,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="2:24">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>95</v>
       </c>
@@ -1670,7 +1704,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="2:24">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>96</v>
       </c>
@@ -1720,7 +1754,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="2:24">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>97</v>
       </c>
@@ -1770,7 +1804,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>98</v>
       </c>
@@ -1820,7 +1854,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="2:24">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>99</v>
       </c>
@@ -1840,7 +1874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:24">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>100</v>
       </c>
@@ -1860,7 +1894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:24">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>101</v>
       </c>
@@ -1880,7 +1914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>102</v>
       </c>
@@ -1900,7 +1934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:24">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
@@ -1920,7 +1954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>104</v>
       </c>
@@ -1940,7 +1974,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:21">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>105</v>
       </c>
@@ -1960,7 +1994,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>106</v>
       </c>
@@ -1980,7 +2014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:21">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>34</v>
       </c>
@@ -2006,7 +2040,7 @@
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +2090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
@@ -2106,7 +2140,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="2:21">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>59</v>
       </c>
@@ -2156,7 +2190,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="2:21">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>60</v>
       </c>
@@ -2206,7 +2240,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="2:21">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
@@ -2256,7 +2290,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="2:21">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>62</v>
       </c>
@@ -2306,7 +2340,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="2:21">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>63</v>
       </c>
@@ -2356,7 +2390,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="2:21">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>64</v>
       </c>
@@ -2406,7 +2440,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="2:21">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
@@ -2456,7 +2490,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="2:21">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>66</v>
       </c>
@@ -2476,7 +2510,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="2:21">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>67</v>
       </c>
@@ -2496,7 +2530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="2:21">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>68</v>
       </c>
@@ -2516,7 +2550,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>69</v>
       </c>
@@ -2536,7 +2570,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>70</v>
       </c>
@@ -2556,7 +2590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>71</v>
       </c>
@@ -2576,7 +2610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>72</v>
       </c>
@@ -2596,7 +2630,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
@@ -2634,21 +2668,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="15" style="1" customWidth="1"/>
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="11" t="s">
         <v>133</v>
@@ -2669,7 +2703,7 @@
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -2722,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>126</v>
       </c>
@@ -2778,7 +2812,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>134</v>
       </c>
@@ -2832,7 +2866,7 @@
       </c>
       <c r="R4" s="12"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>135</v>
       </c>
@@ -2886,7 +2920,7 @@
       </c>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>136</v>
       </c>
@@ -2940,7 +2974,7 @@
       </c>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>137</v>
       </c>
@@ -2996,7 +3030,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>138</v>
       </c>
@@ -3050,7 +3084,7 @@
       </c>
       <c r="R8" s="13"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>139</v>
       </c>
@@ -3104,7 +3138,7 @@
       </c>
       <c r="R9" s="13"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>140</v>
       </c>

</xml_diff>